<commit_message>
Atualização artefato 21 - (Agenda)
Inclusão do depósito de dados "Agenda" no artefato 21 e atualizações nos artefatos 16 e 17 oriundas desta inclusão.
</commit_message>
<xml_diff>
--- a/17 - Lista de Eventos.xlsx
+++ b/17 - Lista de Eventos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Faculdade\3_Semestre\Engenharia de Requisitos\Eng-Soft-EC2A-develop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willians Pavelski\Downloads\Eng-Soft-EC2A-develop\Eng-Soft-EC2A-develop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9A0B3C-90DD-4B97-BC90-C51ECF192DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B512B738-BB89-4601-8B65-CE6888A98B9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4F11F978-06F5-4697-9B62-95608A90EF98}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4F11F978-06F5-4697-9B62-95608A90EF98}"/>
   </bookViews>
   <sheets>
     <sheet name="Eventos" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="89">
   <si>
     <t>Capacidades</t>
   </si>
@@ -295,6 +295,9 @@
   </si>
   <si>
     <t>Toda segunda-feira o Administrador solicita status do serviço</t>
+  </si>
+  <si>
+    <t>Administrador envia agenda técnica de serviço</t>
   </si>
 </sst>
 </file>
@@ -722,9 +725,36 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -745,33 +775,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1089,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6A5D19-EF37-43E1-87F1-23408A5145A4}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,36 +1112,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36" t="s">
+      <c r="C1" s="45"/>
+      <c r="D1" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47" t="s">
+      <c r="G1" s="32"/>
+      <c r="H1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="48"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="33"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
       <c r="F2" s="30" t="s">
         <v>2</v>
       </c>
@@ -1159,13 +1162,13 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="38" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="26">
@@ -1184,9 +1187,9 @@
       <c r="K3" s="29"/>
     </row>
     <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="40"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="6">
         <v>2</v>
       </c>
@@ -1203,9 +1206,9 @@
       <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="40"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="34"/>
       <c r="D5" s="6">
         <v>3</v>
       </c>
@@ -1222,9 +1225,9 @@
       <c r="K5" s="11"/>
     </row>
     <row r="6" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="40"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="6">
         <v>4</v>
       </c>
@@ -1241,9 +1244,9 @@
       <c r="K6" s="11"/>
     </row>
     <row r="7" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="40"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="6">
         <v>5</v>
       </c>
@@ -1260,9 +1263,9 @@
       <c r="K7" s="11"/>
     </row>
     <row r="8" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="40"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="6">
         <v>6</v>
       </c>
@@ -1279,9 +1282,9 @@
       <c r="K8" s="11"/>
     </row>
     <row r="9" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="40" t="s">
+      <c r="A9" s="41"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="34" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="6">
@@ -1300,9 +1303,9 @@
       <c r="K9" s="11"/>
     </row>
     <row r="10" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="40"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="6">
         <v>8</v>
       </c>
@@ -1319,9 +1322,9 @@
       <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="40"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="34"/>
       <c r="D11" s="6">
         <v>9</v>
       </c>
@@ -1338,11 +1341,11 @@
       <c r="K11" s="11"/>
     </row>
     <row r="12" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="41" t="s">
+      <c r="A12" s="41"/>
+      <c r="B12" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="34" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="6">
@@ -1361,9 +1364,9 @@
       <c r="K12" s="12"/>
     </row>
     <row r="13" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="40"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="6">
         <v>11</v>
       </c>
@@ -1380,9 +1383,9 @@
       <c r="K13" s="12"/>
     </row>
     <row r="14" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="40"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="6">
         <v>12</v>
       </c>
@@ -1399,9 +1402,9 @@
       <c r="K14" s="12"/>
     </row>
     <row r="15" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="40"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="6">
         <v>13</v>
       </c>
@@ -1418,9 +1421,9 @@
       <c r="K15" s="12"/>
     </row>
     <row r="16" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="46"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="40"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="6">
         <v>14</v>
       </c>
@@ -1437,9 +1440,9 @@
       <c r="K16" s="11"/>
     </row>
     <row r="17" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="40" t="s">
+      <c r="A17" s="41"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="34" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="6">
@@ -1458,9 +1461,9 @@
       <c r="K17" s="11"/>
     </row>
     <row r="18" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="40"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="6">
         <v>16</v>
       </c>
@@ -1477,11 +1480,11 @@
       <c r="K18" s="11"/>
     </row>
     <row r="19" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
-      <c r="B19" s="32" t="s">
+      <c r="A19" s="41"/>
+      <c r="B19" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="34" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="6">
@@ -1500,9 +1503,9 @@
       <c r="K19" s="11"/>
     </row>
     <row r="20" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="40"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="6">
         <v>18</v>
       </c>
@@ -1519,20 +1522,20 @@
       <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="C21" s="34" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="6">
         <v>19</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="F21" s="20" t="s">
         <v>22</v>
@@ -1544,9 +1547,9 @@
       <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="40"/>
+      <c r="A22" s="43"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="34"/>
       <c r="D22" s="6">
         <v>20</v>
       </c>
@@ -1563,11 +1566,11 @@
       <c r="K22" s="11"/>
     </row>
     <row r="23" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
-      <c r="B23" s="32" t="s">
+      <c r="A23" s="43"/>
+      <c r="B23" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="34" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="6">
@@ -1586,9 +1589,9 @@
       <c r="K23" s="11"/>
     </row>
     <row r="24" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="40"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="34"/>
       <c r="D24" s="6">
         <v>22</v>
       </c>
@@ -1605,9 +1608,9 @@
       <c r="K24" s="11"/>
     </row>
     <row r="25" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="40"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="34"/>
       <c r="D25" s="6">
         <v>23</v>
       </c>
@@ -1624,8 +1627,8 @@
       <c r="K25" s="11"/>
     </row>
     <row r="26" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
-      <c r="B26" s="32"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="35"/>
       <c r="C26" s="23" t="s">
         <v>12</v>
       </c>
@@ -1645,11 +1648,11 @@
       <c r="K26" s="11"/>
     </row>
     <row r="27" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
-      <c r="B27" s="41" t="s">
+      <c r="A27" s="43"/>
+      <c r="B27" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="40" t="s">
+      <c r="C27" s="34" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="6">
@@ -1668,9 +1671,9 @@
       <c r="K27" s="11"/>
     </row>
     <row r="28" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="40"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="34"/>
       <c r="D28" s="6">
         <v>26</v>
       </c>
@@ -1687,13 +1690,13 @@
       <c r="K28" s="11"/>
     </row>
     <row r="29" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="40" t="s">
+      <c r="C29" s="34" t="s">
         <v>11</v>
       </c>
       <c r="D29" s="6">
@@ -1712,9 +1715,9 @@
       <c r="K29" s="11"/>
     </row>
     <row r="30" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="40"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="34"/>
       <c r="D30" s="6">
         <v>28</v>
       </c>
@@ -1731,9 +1734,9 @@
       <c r="K30" s="11"/>
     </row>
     <row r="31" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="40"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="34"/>
       <c r="D31" s="6">
         <v>29</v>
       </c>
@@ -1750,11 +1753,11 @@
       <c r="K31" s="11"/>
     </row>
     <row r="32" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="42"/>
-      <c r="B32" s="41" t="s">
+      <c r="A32" s="37"/>
+      <c r="B32" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="34" t="s">
         <v>11</v>
       </c>
       <c r="D32" s="6">
@@ -1773,9 +1776,9 @@
       <c r="K32" s="11"/>
     </row>
     <row r="33" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="40"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="34"/>
       <c r="D33" s="6">
         <v>31</v>
       </c>
@@ -1792,13 +1795,13 @@
       <c r="K33" s="11"/>
     </row>
     <row r="34" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="40" t="s">
+      <c r="C34" s="34" t="s">
         <v>11</v>
       </c>
       <c r="D34" s="6">
@@ -1817,9 +1820,9 @@
       <c r="K34" s="11"/>
     </row>
     <row r="35" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="40"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="34"/>
       <c r="D35" s="6">
         <v>33</v>
       </c>
@@ -1836,9 +1839,9 @@
       <c r="K35" s="11"/>
     </row>
     <row r="36" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="34"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="40"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="34"/>
       <c r="D36" s="6">
         <v>34</v>
       </c>
@@ -1855,9 +1858,9 @@
       <c r="K36" s="11"/>
     </row>
     <row r="37" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="34"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="40"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="34"/>
       <c r="D37" s="6">
         <v>35</v>
       </c>
@@ -1874,8 +1877,8 @@
       <c r="K37" s="11"/>
     </row>
     <row r="38" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="34"/>
-      <c r="B38" s="32"/>
+      <c r="A38" s="43"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="23" t="s">
         <v>12</v>
       </c>
@@ -1895,11 +1898,11 @@
       <c r="K38" s="11"/>
     </row>
     <row r="39" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="34"/>
-      <c r="B39" s="41" t="s">
+      <c r="A39" s="43"/>
+      <c r="B39" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="C39" s="40"/>
+      <c r="C39" s="34"/>
       <c r="D39" s="6">
         <v>37</v>
       </c>
@@ -1916,9 +1919,9 @@
       <c r="K39" s="11"/>
     </row>
     <row r="40" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="34"/>
-      <c r="B40" s="41"/>
-      <c r="C40" s="40"/>
+      <c r="A40" s="43"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="34"/>
       <c r="D40" s="6">
         <v>38</v>
       </c>
@@ -1935,8 +1938,8 @@
       <c r="K40" s="11"/>
     </row>
     <row r="41" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="34"/>
-      <c r="B41" s="32" t="s">
+      <c r="A41" s="43"/>
+      <c r="B41" s="35" t="s">
         <v>61</v>
       </c>
       <c r="C41" s="24"/>
@@ -1956,8 +1959,8 @@
       <c r="K41" s="11"/>
     </row>
     <row r="42" spans="1:11" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="35"/>
-      <c r="B42" s="33"/>
+      <c r="A42" s="44"/>
+      <c r="B42" s="42"/>
       <c r="C42" s="25"/>
       <c r="D42" s="13">
         <v>40</v>
@@ -1976,23 +1979,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B3:B11"/>
-    <mergeCell ref="A3:A20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C23:C25"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="A34:A42"/>
     <mergeCell ref="E1:E2"/>
@@ -2009,6 +1995,23 @@
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="A21:A28"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B3:B11"/>
+    <mergeCell ref="A3:A20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="C19:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Correções finais (Entrega Geral) - 16/17/21
- Artefato 16 na versão correta e com correção no fluxo de dados "cobrar dados técnicos" -> "cobrança de dados técnicos"
- Artefato 17, correção de "FB" nas duas últimas capacidades
- Artefato 21, inclusão das selfcalls nos processos de cobrança (não eventos).
</commit_message>
<xml_diff>
--- a/17 - Lista de Eventos.xlsx
+++ b/17 - Lista de Eventos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willians Pavelski\Downloads\Eng-Soft-EC2A-develop\Eng-Soft-EC2A-develop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Faculdade\3_Semestre\Engenharia de Requisitos\Eng-Soft-EC2A-develop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B512B738-BB89-4601-8B65-CE6888A98B9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604B58A0-D043-4373-86F6-34E1017D4439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4F11F978-06F5-4697-9B62-95608A90EF98}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="89">
   <si>
     <t>Capacidades</t>
   </si>
@@ -380,7 +380,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -598,14 +598,27 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -617,21 +630,21 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -707,20 +720,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
@@ -746,10 +753,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -774,6 +781,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1092,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6A5D19-EF37-43E1-87F1-23408A5145A4}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,84 +1125,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32" t="s">
+      <c r="G1" s="30"/>
+      <c r="H1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="33"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="31"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="30" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="30" t="s">
+      <c r="I2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="30" t="s">
+      <c r="J2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="24">
         <v>1</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="28"/>
+      <c r="F3" s="26"/>
       <c r="G3" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
-      <c r="K3" s="29"/>
+      <c r="K3" s="27"/>
     </row>
     <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="34"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="6">
         <v>2</v>
       </c>
@@ -1206,9 +1219,9 @@
       <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="34"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="32"/>
       <c r="D5" s="6">
         <v>3</v>
       </c>
@@ -1225,9 +1238,9 @@
       <c r="K5" s="11"/>
     </row>
     <row r="6" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="34"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="32"/>
       <c r="D6" s="6">
         <v>4</v>
       </c>
@@ -1244,9 +1257,9 @@
       <c r="K6" s="11"/>
     </row>
     <row r="7" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="34"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="32"/>
       <c r="D7" s="6">
         <v>5</v>
       </c>
@@ -1263,9 +1276,9 @@
       <c r="K7" s="11"/>
     </row>
     <row r="8" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="34"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="32"/>
       <c r="D8" s="6">
         <v>6</v>
       </c>
@@ -1282,9 +1295,9 @@
       <c r="K8" s="11"/>
     </row>
     <row r="9" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="34" t="s">
+      <c r="A9" s="39"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="32" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="6">
@@ -1303,9 +1316,9 @@
       <c r="K9" s="11"/>
     </row>
     <row r="10" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="34"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="32"/>
       <c r="D10" s="6">
         <v>8</v>
       </c>
@@ -1322,9 +1335,9 @@
       <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="34"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="6">
         <v>9</v>
       </c>
@@ -1341,11 +1354,11 @@
       <c r="K11" s="11"/>
     </row>
     <row r="12" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="36" t="s">
+      <c r="A12" s="39"/>
+      <c r="B12" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="32" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="6">
@@ -1364,9 +1377,9 @@
       <c r="K12" s="12"/>
     </row>
     <row r="13" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="34"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="6">
         <v>11</v>
       </c>
@@ -1383,9 +1396,9 @@
       <c r="K13" s="12"/>
     </row>
     <row r="14" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="34"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="6">
         <v>12</v>
       </c>
@@ -1402,9 +1415,9 @@
       <c r="K14" s="12"/>
     </row>
     <row r="15" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="34"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="32"/>
       <c r="D15" s="6">
         <v>13</v>
       </c>
@@ -1421,9 +1434,9 @@
       <c r="K15" s="12"/>
     </row>
     <row r="16" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="34"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="6">
         <v>14</v>
       </c>
@@ -1440,9 +1453,9 @@
       <c r="K16" s="11"/>
     </row>
     <row r="17" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="34" t="s">
+      <c r="A17" s="39"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="32" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="6">
@@ -1461,9 +1474,9 @@
       <c r="K17" s="11"/>
     </row>
     <row r="18" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="34"/>
+      <c r="A18" s="39"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="6">
         <v>16</v>
       </c>
@@ -1480,11 +1493,11 @@
       <c r="K18" s="11"/>
     </row>
     <row r="19" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="35" t="s">
+      <c r="A19" s="39"/>
+      <c r="B19" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="32" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="6">
@@ -1503,9 +1516,9 @@
       <c r="K19" s="11"/>
     </row>
     <row r="20" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="34"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="6">
         <v>18</v>
       </c>
@@ -1522,13 +1535,13 @@
       <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="32" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="6">
@@ -1547,9 +1560,9 @@
       <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="34"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="32"/>
       <c r="D22" s="6">
         <v>20</v>
       </c>
@@ -1566,11 +1579,11 @@
       <c r="K22" s="11"/>
     </row>
     <row r="23" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
-      <c r="B23" s="35" t="s">
+      <c r="A23" s="41"/>
+      <c r="B23" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="32" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="6">
@@ -1589,9 +1602,9 @@
       <c r="K23" s="11"/>
     </row>
     <row r="24" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="34"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="32"/>
       <c r="D24" s="6">
         <v>22</v>
       </c>
@@ -1608,9 +1621,9 @@
       <c r="K24" s="11"/>
     </row>
     <row r="25" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="43"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="34"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="32"/>
       <c r="D25" s="6">
         <v>23</v>
       </c>
@@ -1627,8 +1640,8 @@
       <c r="K25" s="11"/>
     </row>
     <row r="26" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="43"/>
-      <c r="B26" s="35"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="23" t="s">
         <v>12</v>
       </c>
@@ -1648,11 +1661,11 @@
       <c r="K26" s="11"/>
     </row>
     <row r="27" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="43"/>
-      <c r="B27" s="36" t="s">
+      <c r="A27" s="41"/>
+      <c r="B27" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="32" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="6">
@@ -1671,9 +1684,9 @@
       <c r="K27" s="11"/>
     </row>
     <row r="28" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="43"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="34"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="32"/>
       <c r="D28" s="6">
         <v>26</v>
       </c>
@@ -1690,13 +1703,13 @@
       <c r="K28" s="11"/>
     </row>
     <row r="29" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="32" t="s">
         <v>11</v>
       </c>
       <c r="D29" s="6">
@@ -1715,9 +1728,9 @@
       <c r="K29" s="11"/>
     </row>
     <row r="30" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="37"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="34"/>
+      <c r="A30" s="35"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="32"/>
       <c r="D30" s="6">
         <v>28</v>
       </c>
@@ -1734,9 +1747,9 @@
       <c r="K30" s="11"/>
     </row>
     <row r="31" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="34"/>
+      <c r="A31" s="35"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="32"/>
       <c r="D31" s="6">
         <v>29</v>
       </c>
@@ -1753,11 +1766,11 @@
       <c r="K31" s="11"/>
     </row>
     <row r="32" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="37"/>
-      <c r="B32" s="36" t="s">
+      <c r="A32" s="35"/>
+      <c r="B32" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="32" t="s">
         <v>11</v>
       </c>
       <c r="D32" s="6">
@@ -1776,9 +1789,9 @@
       <c r="K32" s="11"/>
     </row>
     <row r="33" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
-      <c r="B33" s="36"/>
-      <c r="C33" s="34"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="32"/>
       <c r="D33" s="6">
         <v>31</v>
       </c>
@@ -1795,13 +1808,13 @@
       <c r="K33" s="11"/>
     </row>
     <row r="34" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="43" t="s">
+      <c r="A34" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="32" t="s">
         <v>11</v>
       </c>
       <c r="D34" s="6">
@@ -1820,9 +1833,9 @@
       <c r="K34" s="11"/>
     </row>
     <row r="35" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="43"/>
-      <c r="B35" s="35"/>
-      <c r="C35" s="34"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="32"/>
       <c r="D35" s="6">
         <v>33</v>
       </c>
@@ -1839,9 +1852,9 @@
       <c r="K35" s="11"/>
     </row>
     <row r="36" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="43"/>
-      <c r="B36" s="35"/>
-      <c r="C36" s="34"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="32"/>
       <c r="D36" s="6">
         <v>34</v>
       </c>
@@ -1858,9 +1871,9 @@
       <c r="K36" s="11"/>
     </row>
     <row r="37" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="43"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="34"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="32"/>
       <c r="D37" s="6">
         <v>35</v>
       </c>
@@ -1877,8 +1890,8 @@
       <c r="K37" s="11"/>
     </row>
     <row r="38" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="43"/>
-      <c r="B38" s="35"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="33"/>
       <c r="C38" s="23" t="s">
         <v>12</v>
       </c>
@@ -1898,11 +1911,13 @@
       <c r="K38" s="11"/>
     </row>
     <row r="39" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="43"/>
-      <c r="B39" s="36" t="s">
+      <c r="A39" s="41"/>
+      <c r="B39" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C39" s="34"/>
+      <c r="C39" s="32" t="s">
+        <v>11</v>
+      </c>
       <c r="D39" s="6">
         <v>37</v>
       </c>
@@ -1919,9 +1934,9 @@
       <c r="K39" s="11"/>
     </row>
     <row r="40" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="43"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="34"/>
+      <c r="A40" s="41"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="32"/>
       <c r="D40" s="6">
         <v>38</v>
       </c>
@@ -1938,11 +1953,13 @@
       <c r="K40" s="11"/>
     </row>
     <row r="41" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="43"/>
-      <c r="B41" s="35" t="s">
+      <c r="A41" s="41"/>
+      <c r="B41" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="C41" s="24"/>
+      <c r="C41" s="47" t="s">
+        <v>11</v>
+      </c>
       <c r="D41" s="5">
         <v>39</v>
       </c>
@@ -1959,9 +1976,9 @@
       <c r="K41" s="11"/>
     </row>
     <row r="42" spans="1:11" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="44"/>
-      <c r="B42" s="42"/>
-      <c r="C42" s="25"/>
+      <c r="A42" s="42"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="48"/>
       <c r="D42" s="13">
         <v>40</v>
       </c>
@@ -1978,7 +1995,8 @@
       <c r="K42" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="34">
+    <mergeCell ref="C41:C42"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="A34:A42"/>
     <mergeCell ref="E1:E2"/>

</xml_diff>